<commit_message>
add some gismo data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonGismo.xlsx
+++ b/ConfigData/Xlsx/DungeonGismo.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -87,18 +87,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>beast1</t>
-  </si>
-  <si>
-    <t>card5</t>
-  </si>
-  <si>
-    <t>dark1</t>
-  </si>
-  <si>
-    <t>demon1</t>
-  </si>
-  <si>
     <t>hero1</t>
   </si>
   <si>
@@ -109,12 +97,119 @@
   </si>
   <si>
     <t>mercury1</t>
+  </si>
+  <si>
+    <t>creature</t>
+  </si>
+  <si>
+    <t>击杀穷奇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一次击败神兽穷奇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossqiongqi</t>
+  </si>
+  <si>
+    <t>FinishSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务完成</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>难度</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hard</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>快速游戏</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在20步内结束游戏</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成游戏步数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>StepToWin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rival2</t>
+  </si>
+  <si>
+    <t>毫发无伤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>通关时生命值等于最大生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>HpRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命值下限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>head3</t>
+  </si>
+  <si>
+    <t>虫族克星</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>副本中累计击杀100只虫族单位</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击杀单位类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>KillRaceId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击杀单位数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>KillRaceCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>insect1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -320,7 +415,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +604,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor theme="4"/>
       </patternFill>
     </fill>
@@ -777,7 +884,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -812,6 +919,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -859,7 +975,131 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1066,14 +1306,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:E22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A3:E22"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Id" dataDxfId="4"/>
-    <tableColumn id="2" name="Name" dataDxfId="3"/>
-    <tableColumn id="3" name="Descript" dataDxfId="2"/>
-    <tableColumn id="9" name="DungeonId" dataDxfId="1"/>
-    <tableColumn id="4" name="Icon" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:K22" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descript" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{AB12BDFF-9326-4D46-BA2E-0BAA94E8646A}" name="Hard" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DungeonId" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{8D27CF5D-FDC0-443A-AC16-44973C75F048}" name="FinishSceneQuest" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{4B3DB7B6-3B0D-4549-A672-CCEA5684EDA7}" name="StepToWin" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{6431F62F-F02D-47EC-9DB7-24B0AB1933AA}" name="HpRate" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{4A8AAE10-4B60-49BC-AE01-F7456825A1CD}" name="KillRaceId" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{4D9F2E05-F1F9-4282-B583-8ADF1C15E8B5}" name="KillRaceCount" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Icon" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1399,11 +1645,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1411,11 +1657,15 @@
     <col min="1" max="1" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="3"/>
     <col min="3" max="3" width="26.125" style="3" customWidth="1"/>
-    <col min="4" max="5" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="3"/>
+    <col min="4" max="4" width="5.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="3" customWidth="1"/>
+    <col min="7" max="10" width="6" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1426,13 +1676,31 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1443,13 +1711,31 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1460,81 +1746,139 @@
         <v>16</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>45000001</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
         <v>18000001</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>17</v>
+      <c r="F4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>45000002</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D5" s="8">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
         <v>18000001</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>18</v>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10">
+        <v>20</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>45000003</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D6" s="8">
+        <v>6</v>
+      </c>
+      <c r="E6" s="8">
         <v>18000001</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>19</v>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>45000004</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="8">
+        <v>43</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8">
         <v>18000001</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>20</v>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10">
+        <v>4</v>
+      </c>
+      <c r="J7" s="10">
+        <v>100</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>45000005</v>
       </c>
@@ -1544,14 +1888,20 @@
       <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8">
         <v>18000001</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>21</v>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>45000006</v>
       </c>
@@ -1561,14 +1911,20 @@
       <c r="C9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8">
         <v>18000001</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>22</v>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
         <v>45000007</v>
       </c>
@@ -1578,14 +1934,20 @@
       <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8">
         <v>18000001</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>23</v>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
         <v>45000008</v>
       </c>
@@ -1595,14 +1957,20 @@
       <c r="C11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="8"/>
+      <c r="E11" s="8">
         <v>18000001</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>24</v>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
         <v>45000101</v>
       </c>
@@ -1612,14 +1980,20 @@
       <c r="C12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="8"/>
+      <c r="E12" s="8">
         <v>18000101</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
         <v>45000102</v>
       </c>
@@ -1629,14 +2003,20 @@
       <c r="C13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="8"/>
+      <c r="E13" s="8">
         <v>18000101</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="7">
         <v>45000103</v>
       </c>
@@ -1646,14 +2026,20 @@
       <c r="C14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8">
         <v>18000101</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
         <v>45000201</v>
       </c>
@@ -1663,14 +2049,20 @@
       <c r="C15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8">
         <v>18000201</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="7">
         <v>45000202</v>
       </c>
@@ -1680,14 +2072,20 @@
       <c r="C16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8">
         <v>18000201</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="7">
         <v>45000203</v>
       </c>
@@ -1697,14 +2095,20 @@
       <c r="C17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8">
         <v>18000201</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="7">
         <v>45000204</v>
       </c>
@@ -1714,14 +2118,20 @@
       <c r="C18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8">
         <v>18000201</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="8">
         <v>45000301</v>
       </c>
@@ -1731,14 +2141,20 @@
       <c r="C19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="8"/>
+      <c r="E19" s="8">
         <v>18000301</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="8">
         <v>45000302</v>
       </c>
@@ -1748,14 +2164,20 @@
       <c r="C20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="8"/>
+      <c r="E20" s="8">
         <v>18000301</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="8">
         <v>45000303</v>
       </c>
@@ -1765,14 +2187,20 @@
       <c r="C21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="8"/>
+      <c r="E21" s="8">
         <v>18000301</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="8">
         <v>45000304</v>
       </c>
@@ -1782,10 +2210,16 @@
       <c r="C22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="8"/>
+      <c r="E22" s="8">
         <v>18000301</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
begin to deal with the gismo system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonGismo.xlsx
+++ b/ConfigData/Xlsx/DungeonGismo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -141,69 +141,92 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>在20步内结束游戏</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成游戏步数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>StepToWin</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>rival2</t>
   </si>
   <si>
-    <t>毫发无伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>通关时生命值等于最大生命值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>HpRate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>生命值下限</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>head3</t>
   </si>
   <si>
-    <t>虫族克星</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>副本中累计击杀100只虫族单位</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击杀单位类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>KillRaceId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击杀单位数量</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>KillRaceCount</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>insect1</t>
+  </si>
+  <si>
+    <t>任务最后状态</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FinishState</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>reward</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>重复次数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FinishCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>间隔重复次数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FinishContinueCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossqiongqi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在20步击败穷奇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续遇到2条溪流</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>雨季</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river</t>
+  </si>
+  <si>
+    <t>StepCost</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀手</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗获胜场数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>WinCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>累计获得10次战斗胜利</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>先决：步数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -415,7 +438,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -617,6 +640,30 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -884,7 +931,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -928,6 +975,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -975,7 +1040,64 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1080,44 +1202,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1306,20 +1390,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:K22" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descript" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{AB12BDFF-9326-4D46-BA2E-0BAA94E8646A}" name="Hard" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:L22" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A3:L22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descript" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{AB12BDFF-9326-4D46-BA2E-0BAA94E8646A}" name="Hard" dataDxfId="8"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DungeonId" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{8D27CF5D-FDC0-443A-AC16-44973C75F048}" name="FinishSceneQuest" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{4B3DB7B6-3B0D-4549-A672-CCEA5684EDA7}" name="StepToWin" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{6431F62F-F02D-47EC-9DB7-24B0AB1933AA}" name="HpRate" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{4A8AAE10-4B60-49BC-AE01-F7456825A1CD}" name="KillRaceId" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{4D9F2E05-F1F9-4282-B583-8ADF1C15E8B5}" name="KillRaceCount" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Icon" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{E0B19E39-1EC8-49A0-9382-CF9C3227CA62}" name="StepCost" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{8D27CF5D-FDC0-443A-AC16-44973C75F048}" name="FinishSceneQuest" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{424384A6-1E46-4457-B601-8B9839019706}" name="FinishState" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{2342FF29-68C2-4173-984E-516B4E2F32E2}" name="FinishContinueCount" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{426E8935-C16D-4293-AA49-CFF9DFD1F453}" name="FinishCount" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{4A8AAE10-4B60-49BC-AE01-F7456825A1CD}" name="WinCount" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Icon" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1646,10 +1731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1659,13 +1744,16 @@
     <col min="3" max="3" width="26.125" style="3" customWidth="1"/>
     <col min="4" max="4" width="5.625" style="3" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="3" customWidth="1"/>
-    <col min="7" max="10" width="6" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="3"/>
+    <col min="6" max="6" width="4.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="3.875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="6" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1681,26 +1769,29 @@
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>33</v>
-      </c>
       <c r="H1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1716,26 +1807,29 @@
       <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1751,26 +1845,29 @@
       <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="H3" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>45000001</v>
       </c>
@@ -1786,18 +1883,23 @@
       <c r="E4" s="8">
         <v>18000001</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="H4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="10"/>
+      <c r="L4" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>45000002</v>
       </c>
@@ -1805,7 +1907,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D5" s="8">
         <v>2</v>
@@ -1813,26 +1915,33 @@
       <c r="E5" s="8">
         <v>18000001</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10">
+      <c r="F5" s="10">
         <v>20</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="10">
+        <v>1</v>
+      </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="10" t="s">
-        <v>35</v>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>45000003</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D6" s="8">
         <v>6</v>
@@ -1841,25 +1950,28 @@
         <v>18000001</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10">
-        <v>1</v>
-      </c>
-      <c r="I6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10">
+        <v>2</v>
+      </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="10" t="s">
-        <v>41</v>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>45000004</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8">
@@ -1868,17 +1980,16 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="10">
-        <v>4</v>
-      </c>
-      <c r="J7" s="10">
-        <v>100</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>48</v>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10">
+        <v>2</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>45000005</v>
       </c>
@@ -1897,11 +2008,12 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="10"/>
+      <c r="L8" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>45000006</v>
       </c>
@@ -1920,11 +2032,12 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="10"/>
+      <c r="L9" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
         <v>45000007</v>
       </c>
@@ -1943,11 +2056,12 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="10"/>
+      <c r="L10" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
         <v>45000008</v>
       </c>
@@ -1966,11 +2080,12 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="10" t="s">
+      <c r="K11" s="10"/>
+      <c r="L11" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
         <v>45000101</v>
       </c>
@@ -1989,11 +2104,12 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="10" t="s">
+      <c r="K12" s="10"/>
+      <c r="L12" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
         <v>45000102</v>
       </c>
@@ -2012,11 +2128,12 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="10" t="s">
+      <c r="K13" s="10"/>
+      <c r="L13" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" s="7">
         <v>45000103</v>
       </c>
@@ -2035,11 +2152,12 @@
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
-      <c r="K14" s="10" t="s">
+      <c r="K14" s="10"/>
+      <c r="L14" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
         <v>45000201</v>
       </c>
@@ -2058,11 +2176,12 @@
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="10" t="s">
+      <c r="K15" s="10"/>
+      <c r="L15" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="7">
         <v>45000202</v>
       </c>
@@ -2081,11 +2200,12 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="10" t="s">
+      <c r="K16" s="10"/>
+      <c r="L16" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17" s="7">
         <v>45000203</v>
       </c>
@@ -2104,11 +2224,12 @@
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="10" t="s">
+      <c r="K17" s="10"/>
+      <c r="L17" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18" s="7">
         <v>45000204</v>
       </c>
@@ -2127,11 +2248,12 @@
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="10" t="s">
+      <c r="K18" s="10"/>
+      <c r="L18" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19" s="8">
         <v>45000301</v>
       </c>
@@ -2150,11 +2272,12 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="10"/>
+      <c r="L19" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20" s="8">
         <v>45000302</v>
       </c>
@@ -2173,11 +2296,12 @@
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
-      <c r="K20" s="10" t="s">
+      <c r="K20" s="10"/>
+      <c r="L20" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21" s="8">
         <v>45000303</v>
       </c>
@@ -2196,11 +2320,12 @@
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="10" t="s">
+      <c r="K21" s="10"/>
+      <c r="L21" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22" s="8">
         <v>45000304</v>
       </c>
@@ -2219,7 +2344,8 @@
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
-      <c r="K22" s="10" t="s">
+      <c r="K22" s="10"/>
+      <c r="L22" s="10" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix some item bag bug. optimise the dungeon tips
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonGismo.xlsx
+++ b/ConfigData/Xlsx/DungeonGismo.xlsx
@@ -190,10 +190,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>在20步击败穷奇</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>连续遇到2条溪流</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -226,6 +222,10 @@
   </si>
   <si>
     <t>先决：步数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在12步内击败穷奇</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1734,7 +1734,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1770,7 +1770,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>27</v>
@@ -1785,7 +1785,7 @@
         <v>42</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>9</v>
@@ -1846,7 +1846,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>26</v>
@@ -1861,7 +1861,7 @@
         <v>41</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>8</v>
@@ -1907,16 +1907,16 @@
         <v>31</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D5" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5" s="8">
         <v>18000001</v>
       </c>
       <c r="F5" s="10">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>44</v>
@@ -1938,20 +1938,20 @@
         <v>45000003</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E6" s="8">
         <v>18000001</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10">
@@ -1968,12 +1968,14 @@
         <v>45000004</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="8"/>
+        <v>52</v>
+      </c>
+      <c r="D7" s="8">
+        <v>4</v>
+      </c>
       <c r="E7" s="8">
         <v>18000001</v>
       </c>
@@ -1983,7 +1985,7 @@
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>34</v>
@@ -1999,7 +2001,9 @@
       <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
       <c r="E8" s="8">
         <v>18000001</v>
       </c>
@@ -2023,7 +2027,9 @@
       <c r="C9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8">
+        <v>2</v>
+      </c>
       <c r="E9" s="8">
         <v>18000001</v>
       </c>
@@ -2047,7 +2053,9 @@
       <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="8">
+        <v>3</v>
+      </c>
       <c r="E10" s="8">
         <v>18000001</v>
       </c>
@@ -2071,7 +2079,9 @@
       <c r="C11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="8">
+        <v>4</v>
+      </c>
       <c r="E11" s="8">
         <v>18000001</v>
       </c>
@@ -2095,7 +2105,9 @@
       <c r="C12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="8">
+        <v>5</v>
+      </c>
       <c r="E12" s="8">
         <v>18000101</v>
       </c>

</xml_diff>

<commit_message>
new made boss qiongqi and unicorn
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonGismo.xlsx
+++ b/ConfigData/Xlsx/DungeonGismo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -87,25 +87,9 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>hero1</t>
-  </si>
-  <si>
-    <t>head2</t>
-  </si>
-  <si>
-    <t>machine2</t>
-  </si>
-  <si>
-    <t>mercury1</t>
-  </si>
-  <si>
     <t>creature</t>
   </si>
   <si>
-    <t>击杀穷奇</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>第一次击败神兽穷奇</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -137,16 +121,9 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>快速游戏</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>rival2</t>
   </si>
   <si>
-    <t>head3</t>
-  </si>
-  <si>
     <t>insect1</t>
   </si>
   <si>
@@ -190,10 +167,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>连续遇到2条溪流</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>雨季</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -227,6 +200,58 @@
   <si>
     <t>在12步内击败穷奇</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees</t>
+  </si>
+  <si>
+    <t>怀疑人生</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续遇到2次【溪流】</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>累计遇到过8次【丛林】</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>快枪手</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>屠龙人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>另一个传说</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>找到并击败另一只神兽</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossunicorn</t>
+  </si>
+  <si>
+    <t>star</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lv51</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lv41</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>water2</t>
+  </si>
+  <si>
+    <t>tree</t>
   </si>
 </sst>
 </file>
@@ -1734,7 +1759,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1764,28 +1789,28 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>50</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>9</v>
@@ -1802,7 +1827,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>4</v>
@@ -1811,19 +1836,19 @@
         <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>24</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>29</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>3</v>
@@ -1840,28 +1865,28 @@
         <v>16</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I3" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>8</v>
@@ -1872,10 +1897,10 @@
         <v>45000001</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D4" s="8">
         <v>1</v>
@@ -1885,10 +1910,10 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I4" s="10">
         <v>1</v>
@@ -1896,7 +1921,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
@@ -1904,10 +1929,10 @@
         <v>45000002</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D5" s="8">
         <v>5</v>
@@ -1919,10 +1944,10 @@
         <v>12</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I5" s="10">
         <v>1</v>
@@ -1930,7 +1955,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
@@ -1938,10 +1963,10 @@
         <v>45000003</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D6" s="8">
         <v>3</v>
@@ -1951,7 +1976,7 @@
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10">
@@ -1960,7 +1985,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
@@ -1968,10 +1993,10 @@
         <v>45000004</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D7" s="8">
         <v>4</v>
@@ -1988,7 +2013,7 @@
         <v>10</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
@@ -1996,10 +2021,10 @@
         <v>45000005</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
@@ -2008,13 +2033,17 @@
         <v>18000001</v>
       </c>
       <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="J8" s="10">
+        <v>8</v>
+      </c>
       <c r="K8" s="10"/>
       <c r="L8" s="10" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
@@ -2022,25 +2051,31 @@
         <v>45000006</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="D9" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E9" s="8">
         <v>18000001</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="10">
+        <v>1</v>
+      </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
@@ -2066,7 +2101,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
@@ -2092,7 +2127,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
finish the first dungeon
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonGismo.xlsx
+++ b/ConfigData/Xlsx/DungeonGismo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -240,18 +240,39 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>lv51</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>lv41</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>water2</t>
   </si>
   <si>
     <t>tree</t>
+  </si>
+  <si>
+    <t>迷失</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续3次迷失在森林中，没能进入更深处</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>innerforest</t>
+  </si>
+  <si>
+    <t>box</t>
+  </si>
+  <si>
+    <t>走失</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有找到穷奇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossqiongqi2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>duelist2</t>
   </si>
 </sst>
 </file>
@@ -1423,13 +1444,13 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descript" dataDxfId="9"/>
     <tableColumn id="6" xr3:uid="{AB12BDFF-9326-4D46-BA2E-0BAA94E8646A}" name="Hard" dataDxfId="8"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DungeonId" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{E0B19E39-1EC8-49A0-9382-CF9C3227CA62}" name="StepCost" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{8D27CF5D-FDC0-443A-AC16-44973C75F048}" name="FinishSceneQuest" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{424384A6-1E46-4457-B601-8B9839019706}" name="FinishState" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{2342FF29-68C2-4173-984E-516B4E2F32E2}" name="FinishContinueCount" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{426E8935-C16D-4293-AA49-CFF9DFD1F453}" name="FinishCount" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{4A8AAE10-4B60-49BC-AE01-F7456825A1CD}" name="WinCount" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Icon" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{E0B19E39-1EC8-49A0-9382-CF9C3227CA62}" name="StepCost" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{8D27CF5D-FDC0-443A-AC16-44973C75F048}" name="FinishSceneQuest" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{424384A6-1E46-4457-B601-8B9839019706}" name="FinishState" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{2342FF29-68C2-4173-984E-516B4E2F32E2}" name="FinishContinueCount" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{426E8935-C16D-4293-AA49-CFF9DFD1F453}" name="FinishCount" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{4A8AAE10-4B60-49BC-AE01-F7456825A1CD}" name="WinCount" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Icon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1759,7 +1780,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1985,7 +2006,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
@@ -2043,7 +2064,7 @@
       </c>
       <c r="K8" s="10"/>
       <c r="L8" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
@@ -2083,25 +2104,29 @@
         <v>45000007</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="D10" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="8">
         <v>18000001</v>
       </c>
       <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="J10" s="10">
+        <v>3</v>
+      </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
@@ -2109,25 +2134,29 @@
         <v>45000008</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D11" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" s="8">
         <v>18000001</v>
       </c>
       <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="I11" s="10">
+        <v>1</v>
+      </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add some gismo for dungeon
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonGismo.xlsx
+++ b/ConfigData/Xlsx/DungeonGismo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -105,10 +105,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>任务完成</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>难度</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -273,6 +269,97 @@
   </si>
   <si>
     <t>duelist2</t>
+  </si>
+  <si>
+    <t>bossmanwang</t>
+  </si>
+  <si>
+    <t>第一次击败蛮王之灵</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>human1</t>
+  </si>
+  <si>
+    <t>灵魂舞者</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求副本道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求副本道具数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedDungeonItemId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedDungeonItemCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ditaoqi</t>
+  </si>
+  <si>
+    <t>在30步内收集到5个陶器</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>收集者</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lamp1</t>
+  </si>
+  <si>
+    <t>任务名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FinishSceneQuestTag</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成任务分类</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trap</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>nd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续遇到2个机关</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>累计连续解除5次机关</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>item1</t>
+  </si>
+  <si>
+    <t>item2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>有机关</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>机械学家</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -484,7 +571,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -712,8 +799,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -848,6 +947,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -977,7 +1094,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1039,6 +1156,21 @@
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1086,7 +1218,71 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1436,21 +1632,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:L22" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A3:L22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descript" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{AB12BDFF-9326-4D46-BA2E-0BAA94E8646A}" name="Hard" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DungeonId" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{E0B19E39-1EC8-49A0-9382-CF9C3227CA62}" name="StepCost" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{8D27CF5D-FDC0-443A-AC16-44973C75F048}" name="FinishSceneQuest" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{424384A6-1E46-4457-B601-8B9839019706}" name="FinishState" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{2342FF29-68C2-4173-984E-516B4E2F32E2}" name="FinishContinueCount" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{426E8935-C16D-4293-AA49-CFF9DFD1F453}" name="FinishCount" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{4A8AAE10-4B60-49BC-AE01-F7456825A1CD}" name="WinCount" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Icon" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:O22" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A3:O22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descript" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{AB12BDFF-9326-4D46-BA2E-0BAA94E8646A}" name="Hard" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DungeonId" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{E0B19E39-1EC8-49A0-9382-CF9C3227CA62}" name="StepCost" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{8D27CF5D-FDC0-443A-AC16-44973C75F048}" name="FinishSceneQuest" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{47B582CD-3CD2-4B90-8332-2832166A5793}" name="FinishSceneQuestTag" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{424384A6-1E46-4457-B601-8B9839019706}" name="FinishState" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{2342FF29-68C2-4173-984E-516B4E2F32E2}" name="FinishContinueCount" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{426E8935-C16D-4293-AA49-CFF9DFD1F453}" name="FinishCount" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{4A8AAE10-4B60-49BC-AE01-F7456825A1CD}" name="WinCount" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{83DF56F9-EAFA-4CFB-9A37-1E14235CCF75}" name="NeedDungeonItemId" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{088BC0F7-3817-4C1B-A2C9-8DA8A0CC87E7}" name="NeedDungeonItemCount" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Icon" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1777,10 +1976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1792,14 +1991,15 @@
     <col min="5" max="5" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.875" style="3" customWidth="1"/>
     <col min="7" max="7" width="12.625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="3.875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="6" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="3"/>
+    <col min="8" max="8" width="7.25" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.625" style="3" customWidth="1"/>
+    <col min="10" max="11" width="3.875" style="3" customWidth="1"/>
+    <col min="12" max="14" width="6" style="3" customWidth="1"/>
+    <col min="15" max="15" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1810,34 +2010,43 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>32</v>
+        <v>80</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1848,7 +2057,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>4</v>
@@ -1860,22 +2069,31 @@
         <v>19</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>33</v>
+        <v>81</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="23" t="s">
         <v>3</v>
       </c>
+      <c r="N2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1886,39 +2104,48 @@
         <v>16</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>36</v>
+        <v>79</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>45000001</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>18</v>
@@ -1933,27 +2160,30 @@
       <c r="G4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="10">
+      <c r="H4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="10">
         <v>1</v>
       </c>
-      <c r="J4" s="10"/>
       <c r="K4" s="10"/>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>45000002</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="8">
         <v>5</v>
@@ -1965,29 +2195,32 @@
         <v>12</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="10">
+        <v>36</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="10">
         <v>1</v>
       </c>
-      <c r="J5" s="10"/>
       <c r="K5" s="10"/>
-      <c r="L5" s="10" t="s">
-        <v>26</v>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>45000003</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="8">
         <v>3</v>
@@ -1997,27 +2230,30 @@
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="10"/>
-      <c r="I6" s="10">
+      <c r="I6" s="10"/>
+      <c r="J6" s="10">
         <v>2</v>
       </c>
-      <c r="J6" s="10"/>
       <c r="K6" s="10"/>
-      <c r="L6" s="10" t="s">
-        <v>57</v>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>45000004</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="8">
         <v>4</v>
@@ -2030,22 +2266,25 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="10">
+      <c r="K7" s="10"/>
+      <c r="L7" s="10">
         <v>10</v>
       </c>
-      <c r="L7" s="10" t="s">
-        <v>27</v>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>45000005</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
@@ -2055,27 +2294,30 @@
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="10">
+      <c r="J8" s="10"/>
+      <c r="K8" s="10">
         <v>8</v>
       </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10" t="s">
-        <v>58</v>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>45000006</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="D9" s="8">
         <v>5</v>
@@ -2085,29 +2327,32 @@
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="10">
+        <v>1</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="10">
-        <v>1</v>
-      </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
         <v>45000007</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="D10" s="8">
         <v>4</v>
@@ -2117,27 +2362,30 @@
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="10">
+      <c r="J10" s="10"/>
+      <c r="K10" s="10">
         <v>3</v>
       </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10" t="s">
-        <v>62</v>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
         <v>45000008</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="D11" s="8">
         <v>3</v>
@@ -2147,19 +2395,22 @@
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10">
+        <v>1</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10">
-        <v>1</v>
-      </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10" t="s">
-        <v>66</v>
-      </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
         <v>45000101</v>
       </c>
@@ -2181,11 +2432,14 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
         <v>45000102</v>
       </c>
@@ -2205,11 +2459,14 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="7">
         <v>45000103</v>
       </c>
@@ -2229,107 +2486,152 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
         <v>45000201</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="8"/>
+        <v>67</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
       <c r="E15" s="8">
         <v>18000201</v>
       </c>
       <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="G15" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="I15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="10">
+        <v>1</v>
+      </c>
       <c r="K15" s="10"/>
-      <c r="L15" s="10" t="s">
-        <v>15</v>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="7">
         <v>45000202</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="8"/>
+        <v>75</v>
+      </c>
+      <c r="D16" s="8">
+        <v>3</v>
+      </c>
       <c r="E16" s="8">
         <v>18000201</v>
       </c>
-      <c r="F16" s="10"/>
+      <c r="F16" s="10">
+        <v>30</v>
+      </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
-      <c r="L16" s="10" t="s">
-        <v>15</v>
+      <c r="L16" s="10"/>
+      <c r="M16" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="N16" s="25">
+        <v>5</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" s="7">
         <v>45000203</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="8"/>
+        <v>84</v>
+      </c>
+      <c r="D17" s="8">
+        <v>2</v>
+      </c>
       <c r="E17" s="8">
         <v>18000201</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="H17" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
+      <c r="J17" s="10">
+        <v>2</v>
+      </c>
       <c r="K17" s="10"/>
-      <c r="L17" s="10" t="s">
-        <v>15</v>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="7">
         <v>45000204</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="8"/>
+        <v>85</v>
+      </c>
+      <c r="D18" s="8">
+        <v>4</v>
+      </c>
       <c r="E18" s="8">
         <v>18000201</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
+      <c r="H18" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10" t="s">
-        <v>15</v>
+      <c r="K18" s="10">
+        <v>5</v>
+      </c>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" s="8">
         <v>45000301</v>
       </c>
@@ -2349,11 +2651,14 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
-      <c r="L19" s="10" t="s">
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="8">
         <v>45000302</v>
       </c>
@@ -2373,11 +2678,14 @@
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
-      <c r="L20" s="10" t="s">
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" s="8">
         <v>45000303</v>
       </c>
@@ -2397,11 +2705,14 @@
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="10" t="s">
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22" s="8">
         <v>45000304</v>
       </c>
@@ -2421,12 +2732,20 @@
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
-      <c r="L22" s="10" t="s">
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="M16:N16">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(M16))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
add a new story
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonGismo.xlsx
+++ b/ConfigData/Xlsx/DungeonGismo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -260,14 +260,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>没有找到穷奇</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossqiongqi2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>duelist2</t>
   </si>
   <si>
@@ -359,13 +351,21 @@
   </si>
   <si>
     <t>机械学家</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rosemaryfield</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续3次进入【迷迭香田】</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1237,13 +1237,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1618,8 +1611,83 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1632,24 +1700,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A3:O22" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A3:O22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:O22" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
+  <autoFilter ref="A3:O22"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descript" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{AB12BDFF-9326-4D46-BA2E-0BAA94E8646A}" name="Hard" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DungeonId" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{E0B19E39-1EC8-49A0-9382-CF9C3227CA62}" name="StepCost" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{8D27CF5D-FDC0-443A-AC16-44973C75F048}" name="FinishSceneQuest" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{47B582CD-3CD2-4B90-8332-2832166A5793}" name="FinishSceneQuestTag" dataDxfId="0"/>
-    <tableColumn id="12" xr3:uid="{424384A6-1E46-4457-B601-8B9839019706}" name="FinishState" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{2342FF29-68C2-4173-984E-516B4E2F32E2}" name="FinishContinueCount" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{426E8935-C16D-4293-AA49-CFF9DFD1F453}" name="FinishCount" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{4A8AAE10-4B60-49BC-AE01-F7456825A1CD}" name="WinCount" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{83DF56F9-EAFA-4CFB-9A37-1E14235CCF75}" name="NeedDungeonItemId" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{088BC0F7-3817-4C1B-A2C9-8DA8A0CC87E7}" name="NeedDungeonItemCount" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Icon" dataDxfId="4"/>
+    <tableColumn id="1" name="Id" dataDxfId="14"/>
+    <tableColumn id="2" name="Name" dataDxfId="13"/>
+    <tableColumn id="3" name="Descript" dataDxfId="12"/>
+    <tableColumn id="6" name="Hard" dataDxfId="11"/>
+    <tableColumn id="9" name="DungeonId" dataDxfId="10"/>
+    <tableColumn id="16" name="StepCost" dataDxfId="9"/>
+    <tableColumn id="5" name="FinishSceneQuest" dataDxfId="8"/>
+    <tableColumn id="10" name="FinishSceneQuestTag" dataDxfId="7"/>
+    <tableColumn id="12" name="FinishState" dataDxfId="6"/>
+    <tableColumn id="13" name="FinishContinueCount" dataDxfId="5"/>
+    <tableColumn id="14" name="FinishCount" dataDxfId="4"/>
+    <tableColumn id="11" name="WinCount" dataDxfId="3"/>
+    <tableColumn id="7" name="NeedDungeonItemId" dataDxfId="2"/>
+    <tableColumn id="8" name="NeedDungeonItemCount" dataDxfId="1"/>
+    <tableColumn id="4" name="Icon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1663,7 +1731,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1975,11 +2043,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2019,10 +2087,10 @@
         <v>44</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>27</v>
@@ -2037,10 +2105,10 @@
         <v>41</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>9</v>
@@ -2069,7 +2137,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>28</v>
@@ -2116,7 +2184,7 @@
         <v>21</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>29</v>
@@ -2131,10 +2199,10 @@
         <v>42</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>8</v>
@@ -2385,7 +2453,7 @@
         <v>62</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="D11" s="8">
         <v>3</v>
@@ -2395,19 +2463,19 @@
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
@@ -2498,10 +2566,10 @@
         <v>45000201</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" s="8">
         <v>1</v>
@@ -2511,7 +2579,7 @@
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10" t="s">
@@ -2525,7 +2593,7 @@
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
@@ -2533,10 +2601,10 @@
         <v>45000202</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D16" s="8">
         <v>3</v>
@@ -2554,13 +2622,13 @@
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N16" s="25">
         <v>5</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.15">
@@ -2568,10 +2636,10 @@
         <v>45000203</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="8">
         <v>2</v>
@@ -2582,7 +2650,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10">
@@ -2593,7 +2661,7 @@
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
@@ -2601,10 +2669,10 @@
         <v>45000204</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D18" s="8">
         <v>4</v>
@@ -2615,10 +2683,10 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10">
@@ -2628,7 +2696,7 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.15">
@@ -2742,7 +2810,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="M16:N16">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="18" priority="1">
       <formula>LEN(TRIM(M16))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix the dungeon bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonGismo.xlsx
+++ b/ConfigData/Xlsx/DungeonGismo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="94">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -360,6 +360,20 @@
   <si>
     <t>连续3次进入【迷迭香田】</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dark2</t>
+  </si>
+  <si>
+    <t>一线生机</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>到达【森林出口】</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestexit</t>
   </si>
 </sst>
 </file>
@@ -1219,6 +1233,13 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1611,83 +1632,8 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1700,24 +1646,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:O22" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
-  <autoFilter ref="A3:O22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:O23" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A3:O23"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Id" dataDxfId="14"/>
-    <tableColumn id="2" name="Name" dataDxfId="13"/>
-    <tableColumn id="3" name="Descript" dataDxfId="12"/>
-    <tableColumn id="6" name="Hard" dataDxfId="11"/>
-    <tableColumn id="9" name="DungeonId" dataDxfId="10"/>
-    <tableColumn id="16" name="StepCost" dataDxfId="9"/>
-    <tableColumn id="5" name="FinishSceneQuest" dataDxfId="8"/>
-    <tableColumn id="10" name="FinishSceneQuestTag" dataDxfId="7"/>
-    <tableColumn id="12" name="FinishState" dataDxfId="6"/>
-    <tableColumn id="13" name="FinishContinueCount" dataDxfId="5"/>
-    <tableColumn id="14" name="FinishCount" dataDxfId="4"/>
-    <tableColumn id="11" name="WinCount" dataDxfId="3"/>
-    <tableColumn id="7" name="NeedDungeonItemId" dataDxfId="2"/>
-    <tableColumn id="8" name="NeedDungeonItemCount" dataDxfId="1"/>
-    <tableColumn id="4" name="Icon" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="15"/>
+    <tableColumn id="2" name="Name" dataDxfId="14"/>
+    <tableColumn id="3" name="Descript" dataDxfId="13"/>
+    <tableColumn id="6" name="Hard" dataDxfId="12"/>
+    <tableColumn id="9" name="DungeonId" dataDxfId="11"/>
+    <tableColumn id="16" name="StepCost" dataDxfId="10"/>
+    <tableColumn id="5" name="FinishSceneQuest" dataDxfId="9"/>
+    <tableColumn id="10" name="FinishSceneQuestTag" dataDxfId="8"/>
+    <tableColumn id="12" name="FinishState" dataDxfId="7"/>
+    <tableColumn id="13" name="FinishContinueCount" dataDxfId="6"/>
+    <tableColumn id="14" name="FinishCount" dataDxfId="5"/>
+    <tableColumn id="11" name="WinCount" dataDxfId="4"/>
+    <tableColumn id="7" name="NeedDungeonItemId" dataDxfId="3"/>
+    <tableColumn id="8" name="NeedDungeonItemCount" dataDxfId="2"/>
+    <tableColumn id="4" name="Icon" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1731,7 +1677,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2044,10 +1990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2480,36 +2426,40 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
-        <v>45000101</v>
+        <v>45000009</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="D12" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12" s="8">
-        <v>18000101</v>
+        <v>18000001</v>
       </c>
       <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="J12" s="10">
+        <v>1</v>
+      </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
-        <v>45000102</v>
+        <v>45000101</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>12</v>
@@ -2517,7 +2467,9 @@
       <c r="C13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8">
+        <v>5</v>
+      </c>
       <c r="E13" s="8">
         <v>18000101</v>
       </c>
@@ -2536,7 +2488,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="7">
-        <v>45000103</v>
+        <v>45000102</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>12</v>
@@ -2563,119 +2515,113 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
-        <v>45000201</v>
+        <v>45000103</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="8">
-        <v>1</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D15" s="8"/>
       <c r="E15" s="8">
-        <v>18000201</v>
+        <v>18000101</v>
       </c>
       <c r="F15" s="10"/>
-      <c r="G15" s="10" t="s">
-        <v>64</v>
-      </c>
+      <c r="G15" s="10"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J15" s="10">
-        <v>1</v>
-      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="7">
-        <v>45000202</v>
+        <v>45000201</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D16" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" s="8">
         <v>18000201</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="J16" s="10">
+        <v>1</v>
+      </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
-      <c r="M16" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="N16" s="25">
-        <v>5</v>
-      </c>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
       <c r="O16" s="10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" s="7">
-        <v>45000203</v>
+        <v>45000202</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D17" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="8">
         <v>18000201</v>
       </c>
-      <c r="F17" s="10"/>
+      <c r="F17" s="10">
+        <v>30</v>
+      </c>
       <c r="G17" s="10"/>
-      <c r="H17" s="10" t="s">
-        <v>80</v>
-      </c>
+      <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="10">
-        <v>2</v>
-      </c>
+      <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
+      <c r="M17" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="N17" s="25">
+        <v>5</v>
+      </c>
       <c r="O17" s="10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="7">
-        <v>45000204</v>
+        <v>45000203</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E18" s="8">
         <v>18000201</v>
@@ -2685,52 +2631,58 @@
       <c r="H18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="I18" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10">
-        <v>5</v>
-      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10">
+        <v>2</v>
+      </c>
+      <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A19" s="8">
-        <v>45000301</v>
+      <c r="A19" s="7">
+        <v>45000204</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="8"/>
+        <v>83</v>
+      </c>
+      <c r="D19" s="8">
+        <v>4</v>
+      </c>
       <c r="E19" s="8">
-        <v>18000301</v>
+        <v>18000201</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="H19" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
+      <c r="K19" s="10">
+        <v>5</v>
+      </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="8">
-        <v>45000302</v>
-      </c>
-      <c r="B20" s="11" t="s">
+        <v>45000301</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -2755,7 +2707,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" s="8">
-        <v>45000303</v>
+        <v>45000302</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>12</v>
@@ -2782,7 +2734,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22" s="8">
-        <v>45000304</v>
+        <v>45000303</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>12</v>
@@ -2807,11 +2759,38 @@
         <v>15</v>
       </c>
     </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A23" s="8">
+        <v>45000304</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8">
+        <v>18000301</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="M16:N16">
-    <cfRule type="containsBlanks" dxfId="18" priority="1">
-      <formula>LEN(TRIM(M16))=0</formula>
+  <conditionalFormatting sqref="M17:N17">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(M17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new dungeon story mechanical
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonGismo.xlsx
+++ b/ConfigData/Xlsx/DungeonGismo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -373,6 +373,30 @@
   </si>
   <si>
     <t>第一次击败泰达米尔</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>boss</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在远古之路击败3个野蛮人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>远古智慧</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>先决：剧本</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedStory</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1232,7 +1256,33 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1625,13 +1675,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1646,24 +1689,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:O23" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
-  <autoFilter ref="A3:O23"/>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Id" dataDxfId="14"/>
-    <tableColumn id="2" name="Name" dataDxfId="13"/>
-    <tableColumn id="3" name="Descript" dataDxfId="12"/>
-    <tableColumn id="6" name="Hard" dataDxfId="11"/>
-    <tableColumn id="9" name="DungeonId" dataDxfId="10"/>
-    <tableColumn id="16" name="StepCost" dataDxfId="9"/>
-    <tableColumn id="5" name="FinishSceneQuest" dataDxfId="8"/>
-    <tableColumn id="10" name="FinishSceneQuestTag" dataDxfId="7"/>
-    <tableColumn id="12" name="FinishState" dataDxfId="6"/>
-    <tableColumn id="13" name="FinishContinueCount" dataDxfId="5"/>
-    <tableColumn id="14" name="FinishCount" dataDxfId="4"/>
-    <tableColumn id="11" name="WinCount" dataDxfId="3"/>
-    <tableColumn id="7" name="NeedDungeonItemId" dataDxfId="2"/>
-    <tableColumn id="8" name="NeedDungeonItemCount" dataDxfId="1"/>
-    <tableColumn id="4" name="Icon" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:P24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
+  <autoFilter ref="A3:P24"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Id" dataDxfId="16"/>
+    <tableColumn id="2" name="Name" dataDxfId="15"/>
+    <tableColumn id="3" name="Descript" dataDxfId="14"/>
+    <tableColumn id="6" name="Hard" dataDxfId="13"/>
+    <tableColumn id="9" name="DungeonId" dataDxfId="12"/>
+    <tableColumn id="16" name="StepCost" dataDxfId="11"/>
+    <tableColumn id="15" name="NeedStory" dataDxfId="0"/>
+    <tableColumn id="5" name="FinishSceneQuest" dataDxfId="10"/>
+    <tableColumn id="10" name="FinishSceneQuestTag" dataDxfId="9"/>
+    <tableColumn id="12" name="FinishState" dataDxfId="8"/>
+    <tableColumn id="13" name="FinishContinueCount" dataDxfId="7"/>
+    <tableColumn id="14" name="FinishCount" dataDxfId="6"/>
+    <tableColumn id="11" name="WinCount" dataDxfId="5"/>
+    <tableColumn id="7" name="NeedDungeonItemId" dataDxfId="4"/>
+    <tableColumn id="8" name="NeedDungeonItemCount" dataDxfId="3"/>
+    <tableColumn id="4" name="Icon" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1990,10 +2034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2004,16 +2048,17 @@
     <col min="4" max="4" width="5.625" style="3" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.25" style="3" customWidth="1"/>
-    <col min="9" max="9" width="8.625" style="3" customWidth="1"/>
-    <col min="10" max="11" width="3.875" style="3" customWidth="1"/>
-    <col min="12" max="14" width="6" style="3" customWidth="1"/>
-    <col min="15" max="15" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="3"/>
+    <col min="7" max="7" width="9.375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.25" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8.625" style="3" customWidth="1"/>
+    <col min="11" max="12" width="3.875" style="3" customWidth="1"/>
+    <col min="13" max="15" width="6" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2032,35 +2077,38 @@
       <c r="F1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="N1" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="O1" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2079,35 +2127,38 @@
       <c r="F2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>28</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="N2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="O2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -2126,35 +2177,38 @@
       <c r="F3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="M3" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="N3" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="O3" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>45000001</v>
       </c>
@@ -2171,25 +2225,26 @@
         <v>18000001</v>
       </c>
       <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="10"/>
+      <c r="J4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="10">
+      <c r="K4" s="10">
         <v>1</v>
       </c>
-      <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
-      <c r="O4" s="10" t="s">
+      <c r="O4" s="10"/>
+      <c r="P4" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>45000002</v>
       </c>
@@ -2208,25 +2263,26 @@
       <c r="F5" s="10">
         <v>12</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="10"/>
+      <c r="J5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="10">
+      <c r="K5" s="10">
         <v>1</v>
       </c>
-      <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="10"/>
+      <c r="P5" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>45000003</v>
       </c>
@@ -2243,23 +2299,24 @@
         <v>18000001</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="10">
+      <c r="J6" s="10"/>
+      <c r="K6" s="10">
         <v>2</v>
       </c>
-      <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
-      <c r="O6" s="10" t="s">
+      <c r="O6" s="10"/>
+      <c r="P6" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>45000004</v>
       </c>
@@ -2281,16 +2338,17 @@
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
-      <c r="L7" s="10">
+      <c r="L7" s="10"/>
+      <c r="M7" s="10">
         <v>10</v>
       </c>
-      <c r="M7" s="10"/>
       <c r="N7" s="10"/>
-      <c r="O7" s="10" t="s">
+      <c r="O7" s="10"/>
+      <c r="P7" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>45000005</v>
       </c>
@@ -2307,23 +2365,24 @@
         <v>18000001</v>
       </c>
       <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="10">
+      <c r="K8" s="10"/>
+      <c r="L8" s="10">
         <v>8</v>
       </c>
-      <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="10"/>
+      <c r="P8" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>45000006</v>
       </c>
@@ -2340,25 +2399,26 @@
         <v>18000001</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="10"/>
+      <c r="J9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="10">
+      <c r="K9" s="10">
         <v>1</v>
       </c>
-      <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="10" t="s">
+      <c r="O9" s="10"/>
+      <c r="P9" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
         <v>45000007</v>
       </c>
@@ -2375,23 +2435,24 @@
         <v>18000001</v>
       </c>
       <c r="F10" s="10"/>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="10">
+      <c r="K10" s="10"/>
+      <c r="L10" s="10">
         <v>3</v>
       </c>
-      <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="10" t="s">
+      <c r="O10" s="10"/>
+      <c r="P10" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
         <v>45000008</v>
       </c>
@@ -2408,23 +2469,24 @@
         <v>18000001</v>
       </c>
       <c r="F11" s="10"/>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="10"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="10">
+      <c r="J11" s="10"/>
+      <c r="K11" s="10">
         <v>3</v>
       </c>
-      <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="10" t="s">
+      <c r="O11" s="10"/>
+      <c r="P11" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
         <v>45000009</v>
       </c>
@@ -2441,23 +2503,24 @@
         <v>18000001</v>
       </c>
       <c r="F12" s="10"/>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="10"/>
+      <c r="H12" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="H12" s="10"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="10">
+      <c r="J12" s="10"/>
+      <c r="K12" s="10">
         <v>1</v>
       </c>
-      <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="10" t="s">
+      <c r="O12" s="10"/>
+      <c r="P12" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
         <v>45000101</v>
       </c>
@@ -2482,11 +2545,12 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="10" t="s">
+      <c r="O13" s="10"/>
+      <c r="P13" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A14" s="7">
         <v>45000102</v>
       </c>
@@ -2509,11 +2573,12 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
-      <c r="O14" s="10" t="s">
+      <c r="O14" s="10"/>
+      <c r="P14" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
         <v>45000103</v>
       </c>
@@ -2536,11 +2601,12 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
-      <c r="O15" s="10" t="s">
+      <c r="O15" s="10"/>
+      <c r="P15" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A16" s="7">
         <v>45000201</v>
       </c>
@@ -2557,25 +2623,26 @@
         <v>18000201</v>
       </c>
       <c r="F16" s="10"/>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="10"/>
+      <c r="H16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="10"/>
+      <c r="J16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="10">
+      <c r="K16" s="10">
         <v>1</v>
       </c>
-      <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
-      <c r="O16" s="10" t="s">
+      <c r="O16" s="10"/>
+      <c r="P16" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17" s="7">
         <v>45000202</v>
       </c>
@@ -2600,17 +2667,18 @@
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="24" t="s">
+      <c r="M17" s="10"/>
+      <c r="N17" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="N17" s="25">
+      <c r="O17" s="25">
         <v>5</v>
       </c>
-      <c r="O17" s="10" t="s">
+      <c r="P17" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18" s="7">
         <v>45000203</v>
       </c>
@@ -2628,22 +2696,23 @@
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="10"/>
+      <c r="I18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10">
+      <c r="J18" s="10"/>
+      <c r="K18" s="10">
         <v>2</v>
       </c>
-      <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
-      <c r="O18" s="10" t="s">
+      <c r="O18" s="10"/>
+      <c r="P18" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19" s="7">
         <v>45000204</v>
       </c>
@@ -2661,55 +2730,67 @@
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="10"/>
+      <c r="I19" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="J19" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10">
+      <c r="K19" s="10"/>
+      <c r="L19" s="10">
         <v>5</v>
       </c>
-      <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
-      <c r="O19" s="10" t="s">
+      <c r="O19" s="10"/>
+      <c r="P19" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A20" s="8">
-        <v>45000301</v>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A20" s="7">
+        <v>45000205</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="8"/>
+        <v>95</v>
+      </c>
+      <c r="D20" s="8">
+        <v>3</v>
+      </c>
       <c r="E20" s="8">
-        <v>18000301</v>
+        <v>18000201</v>
       </c>
       <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
+      <c r="G20" s="10">
+        <v>47000021</v>
+      </c>
       <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
+      <c r="I20" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
+      <c r="L20" s="10">
+        <v>3</v>
+      </c>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
-      <c r="O20" s="10" t="s">
-        <v>15</v>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21" s="8">
-        <v>45000302</v>
-      </c>
-      <c r="B21" s="11" t="s">
+        <v>45000301</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -2728,13 +2809,14 @@
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
-      <c r="O21" s="10" t="s">
+      <c r="O21" s="10"/>
+      <c r="P21" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22" s="8">
-        <v>45000303</v>
+        <v>45000302</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>12</v>
@@ -2755,13 +2837,14 @@
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
-      <c r="O22" s="10" t="s">
+      <c r="O22" s="10"/>
+      <c r="P22" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23" s="8">
-        <v>45000304</v>
+        <v>45000303</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>12</v>
@@ -2782,15 +2865,44 @@
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
-      <c r="O23" s="10" t="s">
+      <c r="O23" s="10"/>
+      <c r="P23" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A24" s="8">
+        <v>45000304</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8">
+        <v>18000301</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="M17:N17">
-    <cfRule type="containsBlanks" dxfId="18" priority="1">
-      <formula>LEN(TRIM(M17))=0</formula>
+  <conditionalFormatting sqref="N17:O17">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(N17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
optimise the new story
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonGismo.xlsx
+++ b/ConfigData/Xlsx/DungeonGismo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -376,14 +376,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>boss</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>在远古之路击败3个野蛮人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>远古智慧</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -397,6 +389,14 @@
   </si>
   <si>
     <t>NeedStory</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dihunshi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>收集3个野蛮人的魂石</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -609,7 +609,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="43">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -846,6 +846,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1132,7 +1138,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1209,6 +1215,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1256,7 +1265,14 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1275,13 +1291,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1675,6 +1684,13 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1698,16 +1714,16 @@
     <tableColumn id="6" name="Hard" dataDxfId="13"/>
     <tableColumn id="9" name="DungeonId" dataDxfId="12"/>
     <tableColumn id="16" name="StepCost" dataDxfId="11"/>
-    <tableColumn id="15" name="NeedStory" dataDxfId="0"/>
-    <tableColumn id="5" name="FinishSceneQuest" dataDxfId="10"/>
-    <tableColumn id="10" name="FinishSceneQuestTag" dataDxfId="9"/>
-    <tableColumn id="12" name="FinishState" dataDxfId="8"/>
-    <tableColumn id="13" name="FinishContinueCount" dataDxfId="7"/>
-    <tableColumn id="14" name="FinishCount" dataDxfId="6"/>
-    <tableColumn id="11" name="WinCount" dataDxfId="5"/>
-    <tableColumn id="7" name="NeedDungeonItemId" dataDxfId="4"/>
-    <tableColumn id="8" name="NeedDungeonItemCount" dataDxfId="3"/>
-    <tableColumn id="4" name="Icon" dataDxfId="2"/>
+    <tableColumn id="15" name="NeedStory" dataDxfId="10"/>
+    <tableColumn id="5" name="FinishSceneQuest" dataDxfId="9"/>
+    <tableColumn id="10" name="FinishSceneQuestTag" dataDxfId="8"/>
+    <tableColumn id="12" name="FinishState" dataDxfId="7"/>
+    <tableColumn id="13" name="FinishContinueCount" dataDxfId="6"/>
+    <tableColumn id="14" name="FinishCount" dataDxfId="5"/>
+    <tableColumn id="11" name="WinCount" dataDxfId="4"/>
+    <tableColumn id="7" name="NeedDungeonItemId" dataDxfId="3"/>
+    <tableColumn id="8" name="NeedDungeonItemCount" dataDxfId="2"/>
+    <tableColumn id="4" name="Icon" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2037,7 +2053,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2078,7 +2094,7 @@
         <v>44</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>75</v>
@@ -2128,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>19</v>
@@ -2178,7 +2194,7 @@
         <v>39</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>21</v>
@@ -2753,10 +2769,10 @@
         <v>45000205</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D20" s="8">
         <v>3</v>
@@ -2765,23 +2781,19 @@
         <v>18000201</v>
       </c>
       <c r="F20" s="10"/>
-      <c r="G20" s="10">
-        <v>47000021</v>
-      </c>
+      <c r="G20" s="10"/>
       <c r="H20" s="10"/>
-      <c r="I20" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
       <c r="K20" s="10"/>
-      <c r="L20" s="10">
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="O20" s="25">
         <v>3</v>
       </c>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
       <c r="P20" s="10" t="s">
         <v>25</v>
       </c>
@@ -2901,8 +2913,13 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="N17:O17">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="20" priority="2">
       <formula>LEN(TRIM(N17))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N20:O20">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(N20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix some dungeon config error
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/DungeonGismo.xlsx
+++ b/ConfigData/Xlsx/DungeonGismo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -198,9 +198,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees</t>
-  </si>
-  <si>
     <t>怀疑人生</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -397,6 +394,10 @@
   </si>
   <si>
     <t>收集3个野蛮人的魂石</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ftrees</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1266,13 +1267,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1691,8 +1685,83 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1705,25 +1774,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:P24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:P24" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A3:P24"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="Id" dataDxfId="16"/>
-    <tableColumn id="2" name="Name" dataDxfId="15"/>
-    <tableColumn id="3" name="Descript" dataDxfId="14"/>
-    <tableColumn id="6" name="Hard" dataDxfId="13"/>
-    <tableColumn id="9" name="DungeonId" dataDxfId="12"/>
-    <tableColumn id="16" name="StepCost" dataDxfId="11"/>
-    <tableColumn id="15" name="NeedStory" dataDxfId="10"/>
-    <tableColumn id="5" name="FinishSceneQuest" dataDxfId="9"/>
-    <tableColumn id="10" name="FinishSceneQuestTag" dataDxfId="8"/>
-    <tableColumn id="12" name="FinishState" dataDxfId="7"/>
-    <tableColumn id="13" name="FinishContinueCount" dataDxfId="6"/>
-    <tableColumn id="14" name="FinishCount" dataDxfId="5"/>
-    <tableColumn id="11" name="WinCount" dataDxfId="4"/>
-    <tableColumn id="7" name="NeedDungeonItemId" dataDxfId="3"/>
-    <tableColumn id="8" name="NeedDungeonItemCount" dataDxfId="2"/>
-    <tableColumn id="4" name="Icon" dataDxfId="1"/>
+    <tableColumn id="1" name="Id" dataDxfId="15"/>
+    <tableColumn id="2" name="Name" dataDxfId="14"/>
+    <tableColumn id="3" name="Descript" dataDxfId="13"/>
+    <tableColumn id="6" name="Hard" dataDxfId="12"/>
+    <tableColumn id="9" name="DungeonId" dataDxfId="11"/>
+    <tableColumn id="16" name="StepCost" dataDxfId="10"/>
+    <tableColumn id="15" name="NeedStory" dataDxfId="9"/>
+    <tableColumn id="5" name="FinishSceneQuest" dataDxfId="8"/>
+    <tableColumn id="10" name="FinishSceneQuestTag" dataDxfId="7"/>
+    <tableColumn id="12" name="FinishState" dataDxfId="6"/>
+    <tableColumn id="13" name="FinishContinueCount" dataDxfId="5"/>
+    <tableColumn id="14" name="FinishCount" dataDxfId="4"/>
+    <tableColumn id="11" name="WinCount" dataDxfId="3"/>
+    <tableColumn id="7" name="NeedDungeonItemId" dataDxfId="2"/>
+    <tableColumn id="8" name="NeedDungeonItemCount" dataDxfId="1"/>
+    <tableColumn id="4" name="Icon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1737,7 +1806,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2053,7 +2122,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2094,13 +2163,13 @@
         <v>44</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>27</v>
@@ -2115,10 +2184,10 @@
         <v>41</v>
       </c>
       <c r="N1" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="22" t="s">
         <v>67</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>68</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>9</v>
@@ -2144,13 +2213,13 @@
         <v>0</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J2" s="13" t="s">
         <v>28</v>
@@ -2194,13 +2263,13 @@
         <v>39</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>29</v>
@@ -2215,10 +2284,10 @@
         <v>42</v>
       </c>
       <c r="N3" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="21" t="s">
         <v>69</v>
-      </c>
-      <c r="O3" s="21" t="s">
-        <v>70</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>8</v>
@@ -2229,7 +2298,7 @@
         <v>45000001</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>18</v>
@@ -2265,7 +2334,7 @@
         <v>45000002</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>45</v>
@@ -2306,7 +2375,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="8">
         <v>3</v>
@@ -2329,7 +2398,7 @@
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
@@ -2369,10 +2438,10 @@
         <v>45000005</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
@@ -2383,7 +2452,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -2395,7 +2464,7 @@
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.15">
@@ -2403,10 +2472,10 @@
         <v>45000006</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="D9" s="8">
         <v>5</v>
@@ -2417,7 +2486,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10" t="s">
@@ -2431,7 +2500,7 @@
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.15">
@@ -2439,10 +2508,10 @@
         <v>45000007</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="D10" s="8">
         <v>4</v>
@@ -2453,7 +2522,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -2465,7 +2534,7 @@
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.15">
@@ -2473,10 +2542,10 @@
         <v>45000008</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" s="8">
         <v>3</v>
@@ -2487,7 +2556,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -2499,7 +2568,7 @@
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.15">
@@ -2507,10 +2576,10 @@
         <v>45000009</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="D12" s="8">
         <v>2</v>
@@ -2521,7 +2590,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -2533,7 +2602,7 @@
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.15">
@@ -2627,10 +2696,10 @@
         <v>45000201</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" s="8">
         <v>1</v>
@@ -2641,7 +2710,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10" t="s">
@@ -2655,7 +2724,7 @@
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
@@ -2663,10 +2732,10 @@
         <v>45000202</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="8">
         <v>3</v>
@@ -2685,13 +2754,13 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O17" s="25">
         <v>5</v>
       </c>
       <c r="P17" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
@@ -2699,10 +2768,10 @@
         <v>45000203</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" s="8">
         <v>2</v>
@@ -2714,7 +2783,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10">
@@ -2725,7 +2794,7 @@
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
@@ -2733,10 +2802,10 @@
         <v>45000204</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" s="8">
         <v>4</v>
@@ -2748,10 +2817,10 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>80</v>
       </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10">
@@ -2761,7 +2830,7 @@
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
@@ -2769,10 +2838,10 @@
         <v>45000205</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="8">
         <v>3</v>
@@ -2789,7 +2858,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
       <c r="N20" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O20" s="25">
         <v>3</v>
@@ -2918,7 +2987,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:O20">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="19" priority="1">
       <formula>LEN(TRIM(N20))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>